<commit_message>
Update Regulatory Compliance Excel files
- Updated the Regulatory Compliance - Concern and Effectiveness Excel files to incorporate the latest data and insights on regulatory compliance issues.
</commit_message>
<xml_diff>
--- a/data/Section 3/3.6 Regulatory Compliance/24 Regulatory Compliance- Concern.xlsx
+++ b/data/Section 3/3.6 Regulatory Compliance/24 Regulatory Compliance- Concern.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Section 3/3.6 Regulatory Compliance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Survey Report Agent/surveyreport/data/Section 3/3.6 Regulatory Compliance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{03AE1D18-0CC2-49F6-9653-E476B9BBB437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2962E9C-1386-4208-8586-61F8BD9C89FA}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{03AE1D18-0CC2-49F6-9653-E476B9BBB437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{257ECDCC-E15F-4136-B226-E9FBBB9C58E7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FE0B4CBE-84F3-4C9F-82AE-9919CE62AAF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{FE0B4CBE-84F3-4C9F-82AE-9919CE62AAF0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$1001</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$K$1001</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4017" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4019" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Extremely Concerning </t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -253,6 +259,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0263F187-BB10-4321-AA99-4F68C6080D92}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{0263F187-BB10-4321-AA99-4F68C6080D92}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2D25C707-FA0C-4EEB-B27B-6C70156EACE1}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{7E24CE15-0A4A-442B-BA77-6D567D102AF7}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -574,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C8E506-AE50-4E53-89E0-9EA2210012AF}">
   <dimension ref="A1:K1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -35630,66 +35647,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C68BC7E-FD65-4AD5-AE7C-5F657879894E}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>